<commit_message>
Fix many todos, write thanks and abstract first versions
</commit_message>
<xml_diff>
--- a/png/time/Time_spent.xlsx
+++ b/png/time/Time_spent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\FIT\MI\DIP\text\png\time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36632A-18D0-4043-964D-7B407D0B57E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB06413-E9D4-413C-B7CE-9591A7E7308E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CCBD5744-998B-4F34-9DA3-70A2F9CE939E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Analýza</t>
   </si>
@@ -43,6 +43,54 @@
   </si>
   <si>
     <t>Testování</t>
+  </si>
+  <si>
+    <t>Psaní textu</t>
+  </si>
+  <si>
+    <t>říjen 2018</t>
+  </si>
+  <si>
+    <t>listopad 2018</t>
+  </si>
+  <si>
+    <t>prosines 2018</t>
+  </si>
+  <si>
+    <t>leden 2019</t>
+  </si>
+  <si>
+    <t>únor 2019</t>
+  </si>
+  <si>
+    <t>březen 2019</t>
+  </si>
+  <si>
+    <t>duben 2019</t>
+  </si>
+  <si>
+    <t>květen 2019</t>
+  </si>
+  <si>
+    <t>červen 2019</t>
+  </si>
+  <si>
+    <t>červenec 2019</t>
+  </si>
+  <si>
+    <t>srpen 2019</t>
+  </si>
+  <si>
+    <t>září 2019</t>
+  </si>
+  <si>
+    <t>říjen 2019</t>
+  </si>
+  <si>
+    <t>listopad 2019</t>
+  </si>
+  <si>
+    <t>prosinec 2019</t>
   </si>
 </sst>
 </file>
@@ -85,9 +133,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,70 +167,21 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="cs-CZ"/>
-              <a:t>Strávený čas</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="cs-CZ" baseline="0"/>
-              <a:t> na projektu</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.2421578248379426E-2"/>
+          <c:y val="6.2035771667468417E-2"/>
+          <c:w val="0.96859870368224299"/>
+          <c:h val="0.67127073653258651"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -199,7 +198,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -208,75 +207,62 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$B$1:$P$1</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>43374</c:v>
+                  <c:v>říjen 2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43405</c:v>
+                  <c:v>listopad 2018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43435</c:v>
+                  <c:v>prosines 2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43466</c:v>
+                  <c:v>leden 2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43497</c:v>
+                  <c:v>únor 2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43525</c:v>
+                  <c:v>březen 2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43556</c:v>
+                  <c:v>duben 2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43586</c:v>
+                  <c:v>květen 2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43617</c:v>
+                  <c:v>červen 2019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43647</c:v>
+                  <c:v>červenec 2019</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43678</c:v>
+                  <c:v>srpen 2019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43709</c:v>
+                  <c:v>září 2019</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43739</c:v>
+                  <c:v>říjen 2019</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43770</c:v>
+                  <c:v>listopad 2019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>prosinec 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$P$2</c:f>
               <c:numCache>
@@ -329,11 +315,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F815-4239-A90C-20CCEBD32181}"/>
+              <c16:uniqueId val="{00000000-B9FD-40A8-825C-ECC3D6DC7ED6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -352,7 +338,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -361,75 +347,62 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$B$1:$P$1</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>43374</c:v>
+                  <c:v>říjen 2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43405</c:v>
+                  <c:v>listopad 2018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43435</c:v>
+                  <c:v>prosines 2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43466</c:v>
+                  <c:v>leden 2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43497</c:v>
+                  <c:v>únor 2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43525</c:v>
+                  <c:v>březen 2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43556</c:v>
+                  <c:v>duben 2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43586</c:v>
+                  <c:v>květen 2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43617</c:v>
+                  <c:v>červen 2019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43647</c:v>
+                  <c:v>červenec 2019</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43678</c:v>
+                  <c:v>srpen 2019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43709</c:v>
+                  <c:v>září 2019</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43739</c:v>
+                  <c:v>říjen 2019</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43770</c:v>
+                  <c:v>listopad 2019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>prosinec 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$3:$P$3</c:f>
               <c:numCache>
@@ -442,7 +415,7 @@
                   <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.47013888888888888</c:v>
@@ -482,11 +455,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F815-4239-A90C-20CCEBD32181}"/>
+              <c16:uniqueId val="{00000001-B9FD-40A8-825C-ECC3D6DC7ED6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -505,7 +478,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -514,75 +487,62 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$B$1:$P$1</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>43374</c:v>
+                  <c:v>říjen 2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43405</c:v>
+                  <c:v>listopad 2018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43435</c:v>
+                  <c:v>prosines 2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43466</c:v>
+                  <c:v>leden 2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43497</c:v>
+                  <c:v>únor 2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43525</c:v>
+                  <c:v>březen 2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43556</c:v>
+                  <c:v>duben 2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43586</c:v>
+                  <c:v>květen 2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43617</c:v>
+                  <c:v>červen 2019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43647</c:v>
+                  <c:v>červenec 2019</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43678</c:v>
+                  <c:v>srpen 2019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43709</c:v>
+                  <c:v>září 2019</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43739</c:v>
+                  <c:v>říjen 2019</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43770</c:v>
+                  <c:v>listopad 2019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>prosinec 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$4:$P$4</c:f>
               <c:numCache>
@@ -635,11 +595,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F815-4239-A90C-20CCEBD32181}"/>
+              <c16:uniqueId val="{00000002-B9FD-40A8-825C-ECC3D6DC7ED6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -658,7 +618,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -667,75 +627,62 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$B$1:$P$1</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>43374</c:v>
+                  <c:v>říjen 2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43405</c:v>
+                  <c:v>listopad 2018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43435</c:v>
+                  <c:v>prosines 2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43466</c:v>
+                  <c:v>leden 2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43497</c:v>
+                  <c:v>únor 2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43525</c:v>
+                  <c:v>březen 2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43556</c:v>
+                  <c:v>duben 2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43586</c:v>
+                  <c:v>květen 2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43617</c:v>
+                  <c:v>červen 2019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43647</c:v>
+                  <c:v>červenec 2019</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43678</c:v>
+                  <c:v>srpen 2019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43709</c:v>
+                  <c:v>září 2019</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43739</c:v>
+                  <c:v>říjen 2019</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43770</c:v>
+                  <c:v>listopad 2019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>prosinec 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$5:$P$5</c:f>
               <c:numCache>
@@ -748,7 +695,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -788,11 +735,151 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F815-4239-A90C-20CCEBD32181}"/>
+              <c16:uniqueId val="{00000003-B9FD-40A8-825C-ECC3D6DC7ED6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Psaní textu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>říjen 2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>listopad 2018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>prosines 2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>leden 2019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>únor 2019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>březen 2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>duben 2019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>květen 2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>červen 2019</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>červenec 2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>srpen 2019</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>září 2019</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>říjen 2019</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>listopad 2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>prosinec 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>[h]:mm:ss;@</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44861111111111113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16041666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17847222222222223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38541666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1666666666666666E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8749999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31458333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.21180555555555555</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52152777777777781</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.67083333333333339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B9FD-40A8-825C-ECC3D6DC7ED6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -804,11 +891,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="869289728"/>
-        <c:axId val="879736688"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="869289728"/>
+        <c:smooth val="0"/>
+        <c:axId val="876471007"/>
+        <c:axId val="1097683455"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="876471007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,10 +913,12 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -837,8 +927,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -846,11 +936,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-1680000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -865,15 +955,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="879736688"/>
+        <c:crossAx val="1097683455"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="879736688"/>
+        <c:axId val="1097683455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3"/>
+          <c:max val="2.5083290000000003"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -892,20 +986,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="[h]:mm:ss;@" sourceLinked="1"/>
+        <c:numFmt formatCode="[h];@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -914,7 +1002,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -929,9 +1017,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="869289728"/>
+        <c:crossAx val="876471007"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.20833300000000002"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -943,6 +1032,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5261573340274728E-2"/>
+          <c:y val="0.93270742687119623"/>
+          <c:w val="0.90818849207883279"/>
+          <c:h val="4.5314699990223133E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -956,7 +1055,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1058,7 +1157,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1085,8 +1184,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1166,6 +1265,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1176,6 +1280,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1187,7 +1296,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1207,6 +1316,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1219,10 +1331,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1262,23 +1374,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1383,8 +1494,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1516,20 +1627,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1543,17 +1653,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1578,22 +1677,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>40105</xdr:colOff>
+      <xdr:colOff>111672</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>26693</xdr:rowOff>
+      <xdr:rowOff>59119</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>580648</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>107656</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>272761</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>134216</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88E2BA4-4DE6-4AA4-97B2-2A4750BCAA96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A538EA16-61AE-4DA8-A4F6-5ADA329AB1B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,19 +1717,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.01939</cdr:y>
+      <cdr:x>0.049</cdr:x>
+      <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.06645</cdr:x>
-      <cdr:y>0.06321</cdr:y>
+      <cdr:x>0.11567</cdr:x>
+      <cdr:y>0.06275</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF876C11-0EA6-4BD8-B177-7A3B43D6402B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF5088A4-499A-4280-A649-CFFECE8015AE}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -1638,8 +1737,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="108662"/>
-          <a:ext cx="802105" cy="245645"/>
+          <a:off x="380546" y="0"/>
+          <a:ext cx="517791" cy="255728"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1650,116 +1749,24 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="cs-CZ" sz="1100"/>
+            <a:rPr lang="cs-CZ" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
             <a:t>hodin</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.90793</cdr:x>
-      <cdr:y>0.90071</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.97438</cdr:x>
-      <cdr:y>0.94454</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDD873C1-ED2D-4282-864D-B8438D989766}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="10959432" y="5048918"/>
-          <a:ext cx="802105" cy="245645"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="cs-CZ" sz="1100"/>
-            <a:t>měsíc, rok</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2066,113 +2073,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C2F2-6607-4B06-90D1-690A875003F2}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
-        <v>43374</v>
-      </c>
-      <c r="C1" s="1">
-        <v>43405</v>
-      </c>
-      <c r="D1" s="1">
-        <v>43435</v>
-      </c>
-      <c r="E1" s="1">
-        <v>43466</v>
-      </c>
-      <c r="F1" s="1">
-        <v>43497</v>
-      </c>
-      <c r="G1" s="1">
-        <v>43525</v>
-      </c>
-      <c r="H1" s="1">
-        <v>43556</v>
-      </c>
-      <c r="I1" s="1">
-        <v>43586</v>
-      </c>
-      <c r="J1" s="1">
-        <v>43617</v>
-      </c>
-      <c r="K1" s="1">
-        <v>43647</v>
-      </c>
-      <c r="L1" s="1">
-        <v>43678</v>
-      </c>
-      <c r="M1" s="1">
-        <v>43709</v>
-      </c>
-      <c r="N1" s="1">
-        <v>43739</v>
-      </c>
-      <c r="O1" s="1">
-        <v>43770</v>
-      </c>
-      <c r="P1" s="1">
-        <v>43800</v>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.13125000000000001</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.44930555555555557</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.57847222222222217</v>
       </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
         <f>SUM(B2:P2)</f>
         <v>1.1590277777777778</v>
       </c>
@@ -2181,106 +2189,106 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D3" s="3">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.47013888888888888</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.34375</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.32708333333333334</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0.21597222222222223</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>7.6388888888888895E-2</v>
       </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3">
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
         <v>2.6388888888888889E-2</v>
       </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3">
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q5" si="0">SUM(B3:P3)</f>
-        <v>2.3763888888888891</v>
+        <v>2.2097222222222226</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
         <v>1.2499999999999999E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.35347222222222219</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2.4916666666666667</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>2.2972222222222221</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>1.4201388888888888</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>1.4729166666666667</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>1.0854166666666667</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>0.69097222222222221</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>2.1374999999999997</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>1.6506944444444445</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>1.9763888888888888</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>0.14375000000000002</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <f t="shared" si="0"/>
         <v>15.732638888888886</v>
       </c>
@@ -2289,75 +2297,108 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
         <v>9.0277777777777787E-3</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
         <v>0.12222222222222223</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>9.3055555555555558E-2</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>1.1833333333333333</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>1.4215277777777777</v>
+        <v>1.5881944444444445</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.16041666666666668</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.31458333333333333</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="Q6" s="2">
         <f>SUM(Q2:Q5)</f>
-        <v>20.689583333333331</v>
+        <v>20.689583333333328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enrich GUI draft chapter, fix whole text fluence, fix many typos
</commit_message>
<xml_diff>
--- a/png/time/Time_spent.xlsx
+++ b/png/time/Time_spent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\FIT\MI\DIP\text\png\time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB06413-E9D4-413C-B7CE-9591A7E7308E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAB7AE9-EF41-4ED7-A61B-0BB432FFAC0E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CCBD5744-998B-4F34-9DA3-70A2F9CE939E}"/>
   </bookViews>
@@ -424,13 +424,13 @@
                   <c:v>0.34375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32708333333333334</c:v>
+                  <c:v>0.36874999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.21597222222222223</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.3333333333333329E-2</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7.6388888888888895E-2</c:v>
@@ -564,13 +564,13 @@
                   <c:v>0.35347222222222219</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4916666666666667</c:v>
+                  <c:v>2.4499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.2972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4201388888888888</c:v>
+                  <c:v>1.3784722222222223</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.4729166666666667</c:v>
@@ -871,7 +871,7 @@
                   <c:v>0.52152777777777781</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.67083333333333339</c:v>
+                  <c:v>1.2916666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,15 +1677,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>111672</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>59119</xdr:rowOff>
+      <xdr:colOff>100889</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>102251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>272761</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>134216</xdr:rowOff>
+      <xdr:colOff>261978</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177348</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C2F2-6607-4B06-90D1-690A875003F2}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,13 +2205,13 @@
         <v>0.34375</v>
       </c>
       <c r="G3" s="2">
-        <v>0.32708333333333334</v>
+        <v>0.36874999999999997</v>
       </c>
       <c r="H3" s="2">
         <v>0.21597222222222223</v>
       </c>
       <c r="I3" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="J3" s="2">
         <v>7.6388888888888895E-2</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q5" si="0">SUM(B3:P3)</f>
-        <v>2.2097222222222226</v>
+        <v>2.2930555555555556</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2259,13 +2259,13 @@
         <v>0.35347222222222219</v>
       </c>
       <c r="G4" s="2">
-        <v>2.4916666666666667</v>
+        <v>2.4499999999999997</v>
       </c>
       <c r="H4" s="2">
         <v>2.2972222222222221</v>
       </c>
       <c r="I4" s="2">
-        <v>1.4201388888888888</v>
+        <v>1.3784722222222223</v>
       </c>
       <c r="J4" s="2">
         <v>1.4729166666666667</v>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>15.732638888888886</v>
+        <v>15.649305555555554</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2394,11 +2394,11 @@
         <v>0.52152777777777781</v>
       </c>
       <c r="P6" s="2">
-        <v>0.67083333333333339</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="Q6" s="2">
         <f>SUM(Q2:Q5)</f>
-        <v>20.689583333333328</v>
+        <v>20.689583333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing testing output, fix diagrams and time chart
</commit_message>
<xml_diff>
--- a/png/time/Time_spent.xlsx
+++ b/png/time/Time_spent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\FIT\MI\DIP\text\png\time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAB7AE9-EF41-4ED7-A61B-0BB432FFAC0E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEFF643-05A2-4CAE-B01E-59F57419EC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CCBD5744-998B-4F34-9DA3-70A2F9CE939E}"/>
   </bookViews>
@@ -272,19 +272,19 @@
                   <c:v>0.13125000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44930555555555557</c:v>
+                  <c:v>0.61597222222222225</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.57847222222222217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -412,16 +412,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47013888888888888</c:v>
+                  <c:v>0.22013888888888888</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34375</c:v>
+                  <c:v>0.30208333333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.36874999999999997</c:v>
@@ -561,10 +561,10 @@
                   <c:v>1.2499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35347222222222219</c:v>
+                  <c:v>0.22847222222222222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4499999999999997</c:v>
+                  <c:v>2.3666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.2972222222222221</c:v>
@@ -1677,13 +1677,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>100889</xdr:colOff>
+      <xdr:colOff>127559</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>102251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>261978</xdr:colOff>
+      <xdr:colOff>288648</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>177348</xdr:rowOff>
     </xdr:to>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C2F2-6607-4B06-90D1-690A875003F2}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,19 +2139,19 @@
         <v>0.13125000000000001</v>
       </c>
       <c r="C2" s="2">
-        <v>0.44930555555555557</v>
+        <v>0.61597222222222225</v>
       </c>
       <c r="D2" s="2">
         <v>0.57847222222222217</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="Q2" s="2">
         <f>SUM(B2:P2)</f>
-        <v>1.1590277777777778</v>
+        <v>1.8256944444444443</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2193,16 +2193,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="D3" s="2">
         <v>0.25</v>
       </c>
       <c r="E3" s="2">
-        <v>0.47013888888888888</v>
+        <v>0.22013888888888888</v>
       </c>
       <c r="F3" s="2">
-        <v>0.34375</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="G3" s="2">
         <v>0.36874999999999997</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q5" si="0">SUM(B3:P3)</f>
-        <v>2.2930555555555556</v>
+        <v>1.8347222222222219</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2256,10 +2256,10 @@
         <v>1.2499999999999999E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>0.35347222222222219</v>
+        <v>0.22847222222222222</v>
       </c>
       <c r="G4" s="2">
-        <v>2.4499999999999997</v>
+        <v>2.3666666666666667</v>
       </c>
       <c r="H4" s="2">
         <v>2.2972222222222221</v>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>15.649305555555554</v>
+        <v>15.440972222222221</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>